<commit_message>
Finishing the Dispatcher bot for ConocoPhillips project, ready to be tested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\ProductionStatement_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDBE143-958D-4851-9150-710794BCF843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB68A76-2B8E-4A9A-912C-9DF8BB6F9567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -248,6 +248,18 @@
   </si>
   <si>
     <t>EagleFord</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>ConocoPhillips_Files</t>
+  </si>
+  <si>
+    <t>Shared</t>
   </si>
 </sst>
 </file>
@@ -726,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z959"/>
+  <dimension ref="A1:Z961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -774,163 +786,225 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="30">
-      <c r="A3" t="s">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="30">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="8"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="A7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>74</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>44</v>
+      <c r="A9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>46</v>
+        <v>72</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="7"/>
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>50</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>52</v>
+      <c r="A17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>53</v>
+      <c r="A18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1867,6 +1941,8 @@
     <row r="957" ht="14.25" customHeight="1"/>
     <row r="958" ht="14.25" customHeight="1"/>
     <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1879,7 +1955,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Errors fixed and tested, working fine
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\ProductionStatement_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB68A76-2B8E-4A9A-912C-9DF8BB6F9567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E383E-2B4D-4E50-BABA-32A261CE83EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
   <si>
     <t>Name</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>Shared</t>
+  </si>
+  <si>
+    <t>QueuedFolderPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Desktop\ConocoData\Queued Folder</t>
   </si>
 </sst>
 </file>
@@ -405,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -424,6 +430,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +748,7 @@
   <dimension ref="A1:Z961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1006,7 +1013,14 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Changing the Config.xlsx to work with dynamic users
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\ProductionStatement_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2E383E-2B4D-4E50-BABA-32A261CE83EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F311D339-CA4E-4185-A2C3-D288FDF21201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
     <t>QueuedFolderPath</t>
   </si>
   <si>
-    <t>C:\Users\Admin\Desktop\ConocoData\Queued Folder</t>
+    <t>%USERPROFILE%\Desktop\ConocoData\Queued Folder</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,7 +748,7 @@
   <dimension ref="A1:Z961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1021,7 +1021,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="B26" s="2"/>
+    </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Fixing some logic errors
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\ProductionStatement_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F311D339-CA4E-4185-A2C3-D288FDF21201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850924B1-4604-4F61-8066-78C17F654565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,23 +256,23 @@
     <t>OrchestratorQueueFolder</t>
   </si>
   <si>
-    <t>ConocoPhillips_Files</t>
-  </si>
-  <si>
-    <t>Shared</t>
-  </si>
-  <si>
     <t>QueuedFolderPath</t>
   </si>
   <si>
     <t>%USERPROFILE%\Desktop\ConocoData\Queued Folder</t>
+  </si>
+  <si>
+    <t>ConocoPhillipsFiles</t>
+  </si>
+  <si>
+    <t>Conoco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -292,6 +292,13 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -411,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +438,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,7 +756,7 @@
   <dimension ref="A1:Z961"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -798,7 +806,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -830,7 +838,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -857,7 +865,9 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B4" s="15"/>
+    </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
@@ -1015,10 +1025,10 @@
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>